<commit_message>
fix: generate report excel
</commit_message>
<xml_diff>
--- a/public/templates/list_daily_template.xlsx
+++ b/public/templates/list_daily_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j1m-1\OneDrive\Documentos\jim\Quisvar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1382E257-33C8-43F9-BE70-6FA722C05A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D06F892-F877-40C9-85F9-832996F5218C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{2A99DD02-9F49-46A8-8BDA-982B4B360E0E}"/>
   </bookViews>
@@ -455,11 +455,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -804,7 +804,7 @@
   <dimension ref="B3:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -821,18 +821,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
@@ -850,15 +850,15 @@
       <c r="F4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="25"/>
@@ -866,27 +866,13 @@
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="27"/>
-      <c r="G5" s="20">
-        <v>1</v>
-      </c>
-      <c r="H5" s="20">
-        <v>2</v>
-      </c>
-      <c r="I5" s="20">
-        <v>3</v>
-      </c>
-      <c r="J5" s="20">
-        <v>4</v>
-      </c>
-      <c r="K5" s="20">
-        <v>5</v>
-      </c>
-      <c r="L5" s="20">
-        <v>6</v>
-      </c>
-      <c r="M5" s="20">
-        <v>7</v>
-      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
     </row>
     <row r="6" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="21"/>
@@ -1050,13 +1036,13 @@
     <row r="37" s="12" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="B3:M3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="B3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>